<commit_message>
Updated FRED Data Taxonomy and removed fred_scrapping.py
</commit_message>
<xml_diff>
--- a/data/external/FRED/FRED_Data_Taxonomy.xlsx
+++ b/data/external/FRED/FRED_Data_Taxonomy.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stamatis\Desktop\MLCryptoPredictor\MLCryptoPredictor\data\external\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stamatis\Desktop\MLCryptoPredictor\MLCryptoPredictor\data\external\FRED\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EC356D-5F12-4AE0-B84B-AD34076AB458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE702EBF-A0E7-4D16-A72A-AB47CCE213EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -393,10 +393,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -678,11 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A2:AE17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -705,29 +704,29 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:31" ht="21" x14ac:dyDescent="0.4">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
     </row>
@@ -825,7 +824,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:31" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:31" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>27</v>
       </c>
@@ -887,7 +886,7 @@
       <c r="AD9" s="3"/>
       <c r="AE9" s="5"/>
     </row>
-    <row r="10" spans="1:31" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:31" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>37</v>
       </c>
@@ -934,7 +933,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:31" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:31" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>42</v>
       </c>
@@ -981,7 +980,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:31" ht="409.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:31" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>52</v>
       </c>
@@ -1169,7 +1168,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:31" ht="172.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:31" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>70</v>
       </c>
@@ -1264,13 +1263,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A7:O17" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="10">
-      <filters>
-        <filter val="Not Seasonally Adjusted"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A2:O2"/>
   </mergeCells>

</xml_diff>